<commit_message>
- Category wise report implemented
</commit_message>
<xml_diff>
--- a/ResourceManagement/Assets/Reports/Sample-Incident-Report.xlsx
+++ b/ResourceManagement/Assets/Reports/Sample-Incident-Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajen\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ResourceManagement\Assets\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653D51F2-BD28-4C0C-A9CC-1D53ABA54AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22438FA9-6357-413F-851B-327F00355647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{38BC7122-FDDB-46AC-9F2B-DDCAA89ACFD2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IncidentReport" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IncidentReport!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IncidentReport!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Ticket_Number</t>
   </si>
@@ -52,13 +52,16 @@
   </si>
   <si>
     <t>Ticket_Closed_Date</t>
+  </si>
+  <si>
+    <t>Ticket_Category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,13 +82,6 @@
       <color rgb="FF2167AE"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,11 +104,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +425,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -440,6 +435,7 @@
     <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -458,13 +454,15 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{DEAB30FF-F91E-4D4D-823C-E44C61E68320}"/>
+  <autoFilter ref="A1:F1" xr:uid="{DEAB30FF-F91E-4D4D-823C-E44C61E68320}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>